<commit_message>
damage calc almost ready
</commit_message>
<xml_diff>
--- a/data/Pokedex.xlsx
+++ b/data/Pokedex.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\rentals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298119C3-A613-4D95-9A8D-21F8E70F339C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA0C15-F2FB-42BA-8B2B-D87B1162D97D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3510" windowWidth="13305" windowHeight="11700" xr2:uid="{18A36A25-4749-47E9-927D-51BE30537ABE}"/>
+    <workbookView xWindow="-6330" yWindow="2820" windowWidth="13305" windowHeight="11700" activeTab="2" xr2:uid="{18A36A25-4749-47E9-927D-51BE30537ABE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Charmander" sheetId="1" r:id="rId1"/>
+    <sheet name="4" sheetId="1" r:id="rId1"/>
+    <sheet name="99" sheetId="2" r:id="rId2"/>
+    <sheet name="810" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="148">
   <si>
     <t>nat_dex</t>
   </si>
@@ -256,6 +258,225 @@
   </si>
   <si>
     <t>Fire</t>
+  </si>
+  <si>
+    <t>Kingler</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Hyper Cutter</t>
+  </si>
+  <si>
+    <t>Shell Armor</t>
+  </si>
+  <si>
+    <t>Sheer Force</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Ally Switch</t>
+  </si>
+  <si>
+    <t>Amnesia</t>
+  </si>
+  <si>
+    <t>Blizzard</t>
+  </si>
+  <si>
+    <t>Brine</t>
+  </si>
+  <si>
+    <t>Brutal Swing</t>
+  </si>
+  <si>
+    <t>Bubble Beam</t>
+  </si>
+  <si>
+    <t>Crabhammer</t>
+  </si>
+  <si>
+    <t>Dive</t>
+  </si>
+  <si>
+    <t>Flail</t>
+  </si>
+  <si>
+    <t>Giga Impact</t>
+  </si>
+  <si>
+    <t>Guillotine</t>
+  </si>
+  <si>
+    <t>Hail</t>
+  </si>
+  <si>
+    <t>Hammer Arm</t>
+  </si>
+  <si>
+    <t>Harden</t>
+  </si>
+  <si>
+    <t>High Horsepower</t>
+  </si>
+  <si>
+    <t>Hydro Pump</t>
+  </si>
+  <si>
+    <t>Hyper Beam</t>
+  </si>
+  <si>
+    <t>Ice Beam</t>
+  </si>
+  <si>
+    <t>Icy Wind</t>
+  </si>
+  <si>
+    <t>Iron Defense</t>
+  </si>
+  <si>
+    <t>Knock Off</t>
+  </si>
+  <si>
+    <t>Leer</t>
+  </si>
+  <si>
+    <t>Liquidation</t>
+  </si>
+  <si>
+    <t>Mud Shot</t>
+  </si>
+  <si>
+    <t>Night Slash</t>
+  </si>
+  <si>
+    <t>Rain Dance</t>
+  </si>
+  <si>
+    <t>Razor Shell</t>
+  </si>
+  <si>
+    <t>Scald</t>
+  </si>
+  <si>
+    <t>Slam</t>
+  </si>
+  <si>
+    <t>Stomp</t>
+  </si>
+  <si>
+    <t>Stomping Tantrum</t>
+  </si>
+  <si>
+    <t>Superpower</t>
+  </si>
+  <si>
+    <t>Surf</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Water Gun</t>
+  </si>
+  <si>
+    <t>Whirlpool</t>
+  </si>
+  <si>
+    <t>Wide Guard</t>
+  </si>
+  <si>
+    <t>X-Scissor</t>
+  </si>
+  <si>
+    <t>Grookey</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Overgrow</t>
+  </si>
+  <si>
+    <t>Grassy Surge</t>
+  </si>
+  <si>
+    <t>Assurance</t>
+  </si>
+  <si>
+    <t>Branch Poke</t>
+  </si>
+  <si>
+    <t>Drain Punch</t>
+  </si>
+  <si>
+    <t>Endeavor</t>
+  </si>
+  <si>
+    <t>Energy Ball</t>
+  </si>
+  <si>
+    <t>Fake Out</t>
+  </si>
+  <si>
+    <t>Focus Energy</t>
+  </si>
+  <si>
+    <t>Giga Drain</t>
+  </si>
+  <si>
+    <t>Grass Knot</t>
+  </si>
+  <si>
+    <t>Grass Pledge</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Leech Seed</t>
+  </si>
+  <si>
+    <t>Low Kick</t>
+  </si>
+  <si>
+    <t>Magical Leaf</t>
+  </si>
+  <si>
+    <t>Nature Power</t>
+  </si>
+  <si>
+    <t>Razor Leaf</t>
+  </si>
+  <si>
+    <t>Screech</t>
+  </si>
+  <si>
+    <t>Solar Beam</t>
+  </si>
+  <si>
+    <t>Solar Blade</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Taunt</t>
+  </si>
+  <si>
+    <t>Uproar</t>
+  </si>
+  <si>
+    <t>U-turn</t>
+  </si>
+  <si>
+    <t>Wood Hammer</t>
+  </si>
+  <si>
+    <t>Worry Seed</t>
   </si>
 </sst>
 </file>
@@ -609,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA46D35-D2D5-4E0F-B85C-3DC7DE072EF2}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,4 +1210,715 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED34C492-6EEC-4373-A84A-377855CF46FB}">
+  <dimension ref="A1:I60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>75</v>
+      </c>
+      <c r="I7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6087DC7F-3855-4303-8B24-48AC98CA7824}">
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>810</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>